<commit_message>
Added more standard bracket templates for 2, 4 people divisions. Now first line is filled in as well.
</commit_message>
<xml_diff>
--- a/Templates/BracketTemplate.xlsx
+++ b/Templates/BracketTemplate.xlsx
@@ -5,14 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Taekwondo\SpringOpen\Templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Taekwondo\SpringOpen\SpringOpenBracketAutomator\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="2-Person" sheetId="5" r:id="rId1"/>
+    <sheet name="4-Person" sheetId="4" r:id="rId2"/>
+    <sheet name="8-Person" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="12">
   <si>
     <t>Ring</t>
   </si>
@@ -83,7 +85,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -182,11 +184,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -198,6 +211,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -220,15 +234,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:colOff>47626</xdr:colOff>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>904875</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -237,8 +251,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1" flipV="1">
-          <a:off x="2743200" y="3276600"/>
-          <a:ext cx="2657475" cy="1866900"/>
+          <a:off x="2714626" y="3086100"/>
+          <a:ext cx="2971799" cy="1857375"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -270,15 +284,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:colOff>57151</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:colOff>923925</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -287,8 +301,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="2781300" y="2085975"/>
-          <a:ext cx="2657475" cy="1905000"/>
+          <a:off x="2724151" y="1905000"/>
+          <a:ext cx="2981324" cy="1885950"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -583,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M33"/>
+  <dimension ref="B1:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,9 +611,10 @@
     <col min="4" max="4" width="13.5703125" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" customWidth="1"/>
     <col min="6" max="6" width="8.85546875" customWidth="1"/>
-    <col min="7" max="7" width="7.140625" customWidth="1"/>
-    <col min="8" max="8" width="6.85546875" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.5703125" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" customWidth="1"/>
     <col min="11" max="11" width="6.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -642,112 +657,663 @@
       </c>
       <c r="M2" s="4"/>
     </row>
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="9"/>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="10"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J27" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="4.5703125" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" customWidth="1"/>
+    <col min="11" max="11" width="6.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="L1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="4"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M3" s="4"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E8" s="5"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E9" s="6"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="9"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C10" s="5"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="6"/>
+      <c r="G10" s="9"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C11" s="6"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="6"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C12" s="6"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="6"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="9"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="3"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="3"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="3"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="3"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="10"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="9"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B17" s="3"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B18" s="3"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="3"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="3"/>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="3"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="3"/>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="3"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="3"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="6"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="10"/>
+      <c r="K22" s="3"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="E23" s="6"/>
+      <c r="G23" s="9"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="E24" s="6"/>
+      <c r="G24" s="9"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="10"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J27" s="3"/>
+    </row>
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>10</v>
+      </c>
+      <c r="I30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M34"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="4.5703125" customWidth="1"/>
+    <col min="8" max="8" width="5.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" customWidth="1"/>
+    <col min="11" max="11" width="6.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1"/>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="L1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="4"/>
+    </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="L3" t="s">
         <v>9</v>
       </c>
-      <c r="M3" s="1"/>
+      <c r="M3" s="4"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="F5" s="5"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="8"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="G6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="9"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="F7" s="5"/>
-      <c r="G7" s="8"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="8"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E8" s="1"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="9"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="9"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E9" s="5"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="8"/>
+      <c r="E9" s="6"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="9"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="E10" s="6"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="3"/>
+      <c r="D10" s="10"/>
       <c r="I10" s="9"/>
+      <c r="J10" s="1"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D11" s="1"/>
+      <c r="D11" s="11"/>
       <c r="E11" s="6"/>
+      <c r="G11" s="1"/>
       <c r="H11" s="3"/>
       <c r="I11" s="9"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="8"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D12" s="5"/>
+      <c r="D12" s="6"/>
       <c r="E12" s="6"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="3"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="8"/>
       <c r="I12" s="9"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="8"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="9"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="1"/>
+      <c r="C13" s="3"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="9"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="10"/>
       <c r="J13" s="3"/>
       <c r="K13" s="9"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+      <c r="C14" s="2"/>
       <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
       <c r="F14" s="6"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="10"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="9"/>
       <c r="J14" s="3"/>
       <c r="K14" s="9"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
-      <c r="C15" s="2"/>
+      <c r="B15" s="6"/>
       <c r="D15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="9"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="10"/>
       <c r="J15" s="3"/>
       <c r="K15" s="9"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" s="6"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="6"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="10"/>
+      <c r="D16" s="7"/>
       <c r="J16" s="3"/>
       <c r="K16" s="9"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>
       <c r="C17" s="3"/>
-      <c r="D17" s="7"/>
       <c r="J17" s="3"/>
       <c r="K17" s="9"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
       <c r="B18" s="6"/>
       <c r="C18" s="3"/>
       <c r="J18" s="3"/>
       <c r="K18" s="9"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="1"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
       <c r="B19" s="6"/>
       <c r="C19" s="3"/>
       <c r="J19" s="3"/>
       <c r="K19" s="9"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="1"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B20" s="6"/>
@@ -758,63 +1324,64 @@
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B21" s="6"/>
       <c r="C21" s="3"/>
+      <c r="D21" s="5"/>
+      <c r="G21" s="1"/>
       <c r="J21" s="3"/>
       <c r="K21" s="9"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B22" s="6"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="5"/>
-      <c r="G22" s="1"/>
+      <c r="D22" s="6"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="8"/>
       <c r="J22" s="3"/>
       <c r="K22" s="9"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B23" s="6"/>
-      <c r="C23" s="3"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="1"/>
       <c r="D23" s="6"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="8"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="9"/>
       <c r="J23" s="3"/>
       <c r="K23" s="9"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="7"/>
-      <c r="C24" s="1"/>
       <c r="D24" s="6"/>
-      <c r="E24" s="1"/>
+      <c r="E24" s="5"/>
       <c r="F24" s="6"/>
-      <c r="G24" s="9"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="8"/>
       <c r="J24" s="3"/>
       <c r="K24" s="9"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D25" s="6"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="3"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="9"/>
       <c r="K25" s="9"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D26" s="6"/>
+      <c r="D26" s="7"/>
       <c r="E26" s="6"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="10"/>
       <c r="H26" s="3"/>
       <c r="I26" s="9"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="9"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="10"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="D27" s="7"/>
       <c r="E27" s="6"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="9"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="10"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E28" s="6"/>
@@ -825,30 +1392,32 @@
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E29" s="6"/>
       <c r="F29" s="5"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="3"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="8"/>
       <c r="I29" s="9"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E30" s="7"/>
       <c r="F30" s="6"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="1"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="9"/>
       <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F31" s="6"/>
-      <c r="G31" s="9"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="9"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F32" s="7"/>
-      <c r="G32" s="10"/>
-    </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+      <c r="G32" s="1"/>
+      <c r="H32" s="10"/>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
         <v>10</v>
       </c>
-      <c r="K33" t="s">
+      <c r="J34" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Byes included in bracket sheet.
</commit_message>
<xml_diff>
--- a/Templates/BracketTemplate.xlsx
+++ b/Templates/BracketTemplate.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8145" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="2-Person" sheetId="5" r:id="rId1"/>
@@ -599,7 +599,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
@@ -856,7 +856,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -931,19 +931,16 @@
       <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C10" s="5"/>
-      <c r="D10" s="2"/>
       <c r="E10" s="6"/>
       <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C11" s="6"/>
-      <c r="D11" s="3"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="2"/>
       <c r="E11" s="6"/>
       <c r="G11" s="9"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="8"/>
+      <c r="I11" s="8"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C12" s="6"/>
@@ -951,8 +948,7 @@
       <c r="E12" s="6"/>
       <c r="G12" s="9"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="9"/>
+      <c r="I12" s="9"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" s="3"/>
@@ -962,8 +958,7 @@
       <c r="F13" s="1"/>
       <c r="G13" s="10"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="9"/>
+      <c r="I13" s="9"/>
       <c r="K13" s="3"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -974,8 +969,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="9"/>
+      <c r="I14" s="9"/>
       <c r="K14" s="3"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
@@ -986,8 +980,7 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="9"/>
+      <c r="I15" s="9"/>
       <c r="K15" s="3"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -999,11 +992,11 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="7"/>
+      <c r="I16" s="9"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
+      <c r="M16" s="3"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
@@ -1013,8 +1006,7 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="3"/>
-      <c r="J17" s="9"/>
+      <c r="I17" s="9"/>
       <c r="K17" s="3"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
@@ -1025,8 +1017,7 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="9"/>
+      <c r="I18" s="9"/>
       <c r="K18" s="3"/>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
@@ -1034,8 +1025,7 @@
       <c r="C19" s="6"/>
       <c r="D19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="3"/>
-      <c r="J19" s="9"/>
+      <c r="I19" s="9"/>
       <c r="K19" s="3"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
@@ -1046,8 +1036,7 @@
       <c r="F20" s="2"/>
       <c r="G20" s="8"/>
       <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="9"/>
+      <c r="I20" s="9"/>
       <c r="K20" s="3"/>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
@@ -1058,8 +1047,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="9"/>
       <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="9"/>
+      <c r="I21" s="9"/>
       <c r="K21" s="3"/>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
@@ -1069,8 +1057,7 @@
       <c r="E22" s="6"/>
       <c r="G22" s="9"/>
       <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="10"/>
+      <c r="I22" s="10"/>
       <c r="K22" s="3"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
@@ -1135,8 +1122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>